<commit_message>
UI Run test based of Tags - Krishnaveni Vivekanandan
</commit_message>
<xml_diff>
--- a/src/test/resources/FHEO-Testdata.xlsx
+++ b/src/test/resources/FHEO-Testdata.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\krish\IdeaProjects\formservice-testing\src\test\resources\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{49B521AA-088D-41DC-B075-0EE2F0483B2D}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F011B5E9-45CE-48C3-8AC8-F0701B30165F}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-96" yWindow="-96" windowWidth="23232" windowHeight="12552" tabRatio="474" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -210,13 +210,13 @@
     <t>Akil1@gmail.com</t>
   </si>
   <si>
-    <t>Krish - Auto1</t>
-  </si>
-  <si>
     <t>Updik1</t>
   </si>
   <si>
-    <t>John - Auto1</t>
+    <t>John1</t>
+  </si>
+  <si>
+    <t>Krishnaveni - Auto1</t>
   </si>
 </sst>
 </file>
@@ -1162,7 +1162,7 @@
       <pane xSplit="3" ySplit="1" topLeftCell="D2" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="E4" sqref="E4"/>
+      <selection pane="bottomRight" activeCell="F9" sqref="F9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.55000000000000004"/>
@@ -1175,7 +1175,7 @@
     <col min="6" max="6" width="5.734375" style="5" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="5.15625" style="5" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="28.5234375" style="6" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="12.5234375" style="8" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="17.05078125" style="8" bestFit="1" customWidth="1"/>
     <col min="10" max="10" width="12.26171875" style="8" bestFit="1" customWidth="1"/>
     <col min="11" max="11" width="14.68359375" style="8" bestFit="1" customWidth="1"/>
     <col min="12" max="12" width="16.1015625" style="8" bestFit="1" customWidth="1"/>
@@ -1343,7 +1343,7 @@
         <v>7</v>
       </c>
       <c r="I2" s="8" t="s">
-        <v>58</v>
+        <v>60</v>
       </c>
       <c r="J2" s="8" t="s">
         <v>54</v>
@@ -1382,10 +1382,10 @@
         <v>27</v>
       </c>
       <c r="V2" s="13" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="W2" s="13" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="X2" s="13">
         <v>2224568749</v>
@@ -1434,12 +1434,11 @@
   <autoFilter ref="A1:AK2" xr:uid="{4C97160D-48E6-4400-8B65-A7CABC8765FE}"/>
   <phoneticPr fontId="18" type="noConversion"/>
   <hyperlinks>
-    <hyperlink ref="Y2" r:id="rId1" xr:uid="{09BE1A2B-927E-47C2-BCE0-52DE6DA62D79}"/>
-    <hyperlink ref="AK2" r:id="rId2" xr:uid="{61755138-C074-448D-BA0F-EB4A675CB29B}"/>
-    <hyperlink ref="M2" r:id="rId3" xr:uid="{8CF6E716-7945-4E64-B583-E92A3F117F40}"/>
-    <hyperlink ref="M2" r:id="rId4" xr:uid="{01708F0C-E245-47DC-9993-020267BF28AF}"/>
+    <hyperlink ref="Y2" r:id="rId1" xr:uid="{ABA2AC56-F1FD-46F7-8D70-55E0BDB9C7EE}"/>
+    <hyperlink ref="AK2" r:id="rId2" xr:uid="{D5425F91-5FBA-49E3-B1CA-57937BE67630}"/>
+    <hyperlink ref="M2" r:id="rId3" xr:uid="{9B372730-10A7-495D-BFC4-9C55BC7ECB17}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" r:id="rId5"/>
+  <pageSetup orientation="portrait" r:id="rId4"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Updated all Specs for accessibility validations
</commit_message>
<xml_diff>
--- a/src/test/resources/FHEO-Testdata.xlsx
+++ b/src/test/resources/FHEO-Testdata.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\krish\IdeaProjects\formservice-testing\src\test\resources\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F011B5E9-45CE-48C3-8AC8-F0701B30165F}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C53B3349-F1FD-44E6-B6C0-BA6C70BCCB32}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-96" yWindow="-96" windowWidth="23232" windowHeight="12552" tabRatio="474" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -216,7 +216,7 @@
     <t>John1</t>
   </si>
   <si>
-    <t>Krishnaveni - Auto1</t>
+    <t>Krish - Auto1</t>
   </si>
 </sst>
 </file>
@@ -1162,7 +1162,7 @@
       <pane xSplit="3" ySplit="1" topLeftCell="D2" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="F9" sqref="F9"/>
+      <selection pane="bottomRight" activeCell="G11" sqref="G11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.55000000000000004"/>
@@ -1434,9 +1434,9 @@
   <autoFilter ref="A1:AK2" xr:uid="{4C97160D-48E6-4400-8B65-A7CABC8765FE}"/>
   <phoneticPr fontId="18" type="noConversion"/>
   <hyperlinks>
-    <hyperlink ref="Y2" r:id="rId1" xr:uid="{ABA2AC56-F1FD-46F7-8D70-55E0BDB9C7EE}"/>
-    <hyperlink ref="AK2" r:id="rId2" xr:uid="{D5425F91-5FBA-49E3-B1CA-57937BE67630}"/>
-    <hyperlink ref="M2" r:id="rId3" xr:uid="{9B372730-10A7-495D-BFC4-9C55BC7ECB17}"/>
+    <hyperlink ref="Y2" r:id="rId1" xr:uid="{CE7DDBE2-AC8A-4020-8ABE-30015308F4AC}"/>
+    <hyperlink ref="AK2" r:id="rId2" xr:uid="{6DDDD816-E48F-4737-A2C4-5754126D1CE7}"/>
+    <hyperlink ref="M2" r:id="rId3" xr:uid="{62025BB8-52D1-4AE5-8ADD-BCE2661AC456}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId4"/>

</xml_diff>